<commit_message>
feat: add grader exam problems
</commit_message>
<xml_diff>
--- a/PL-Problem-List/database/csv/00-problem-list.xlsx
+++ b/PL-Problem-List/database/csv/00-problem-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College Year 1\2110101 COM PROG\COM-PROG\PL-Problem-List\database\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College-Year-1\2110101-COM-PROG\COM-PROG\PL-Problem-List\database\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503B0BBF-B42F-4A54-90CD-73075ED95EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3921A0E8-31D3-4950-BBAC-5C1A90CB5B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="13" activeTab="15" xr2:uid="{7CE59BEB-4450-41B6-873A-7F0FF7381052}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="22" activeTab="24" xr2:uid="{7CE59BEB-4450-41B6-873A-7F0FF7381052}"/>
   </bookViews>
   <sheets>
     <sheet name="00-intro" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,15 @@
     <sheet name="p1-practice" sheetId="14" r:id="rId14"/>
     <sheet name="p2-practice" sheetId="15" r:id="rId15"/>
     <sheet name="p3-practice" sheetId="16" r:id="rId16"/>
+    <sheet name="g6501-exam" sheetId="18" r:id="rId17"/>
+    <sheet name="g6502-exam" sheetId="19" r:id="rId18"/>
+    <sheet name="g6503-exam" sheetId="20" r:id="rId19"/>
+    <sheet name="g6601-exam" sheetId="21" r:id="rId20"/>
+    <sheet name="g6602-exam" sheetId="22" r:id="rId21"/>
+    <sheet name="g6603-exam" sheetId="23" r:id="rId22"/>
+    <sheet name="g6701-exam" sheetId="24" r:id="rId23"/>
+    <sheet name="g6702-exam" sheetId="25" r:id="rId24"/>
+    <sheet name="g6703-exam" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="749">
   <si>
     <t>code</t>
   </si>
@@ -1399,6 +1408,894 @@
   </si>
   <si>
     <t>NumPy Functions</t>
+  </si>
+  <si>
+    <t>2565_1_Q1_01</t>
+  </si>
+  <si>
+    <t>2565_1_Q1_02</t>
+  </si>
+  <si>
+    <t>2565_1_Q1_03</t>
+  </si>
+  <si>
+    <t>2565_1_Q2_01</t>
+  </si>
+  <si>
+    <t>2565_1_Q3_01</t>
+  </si>
+  <si>
+    <t>2565_1_Q2_02</t>
+  </si>
+  <si>
+    <t>2565_1_Q2_03</t>
+  </si>
+  <si>
+    <t>2565_1_Q3_02</t>
+  </si>
+  <si>
+    <t>2565_1_Q3_03</t>
+  </si>
+  <si>
+    <t>Flowchart</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1FXMD_zb9kZY0yza5yGkKEjzhIsln3957/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Multiplexer</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1NuVGKMXHgLQnZ5uYt9max7ulUrsu_2iP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Simple Expression Calculator</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1lVVt7vIHTU--47wxWlmma9nAeVPlxhKd/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Scrabble</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1X6OZDtOLyN39IAgno2ZU1lD7gL25xOpo/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14nVgkqWfDCmAo63yftuhC75UoOSFs9Xi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Y3ZGwib7W2vyC9boj5bUja5Bn7x4YKRV/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Color Splash</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1F26AfX7ZdT7tbOQrNPDPe9K53HqM6b1w/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Group Stage</t>
+  </si>
+  <si>
+    <t>Graduation Ceremony</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1WBB8TOkW_fw3vlitH2TXXcxpklcce0la/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1SPMt7LOB8ThKCUKVqYJX3_a5lpx71_bv/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>APEC Headache</t>
+  </si>
+  <si>
+    <t>2565_2_Q1_01</t>
+  </si>
+  <si>
+    <t>2565_2_Q1_02</t>
+  </si>
+  <si>
+    <t>2565_2_Q1_03</t>
+  </si>
+  <si>
+    <t>2565_2_Q2_01</t>
+  </si>
+  <si>
+    <t>2565_2_Q2_02</t>
+  </si>
+  <si>
+    <t>2565_2_Q2_03</t>
+  </si>
+  <si>
+    <t>2565_2_Q3_01</t>
+  </si>
+  <si>
+    <t>2565_2_Q3_02</t>
+  </si>
+  <si>
+    <t>2565_2_Q3_03</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13yV-9L1WZIbXhRva2IoDF_BxYCrykC7h/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Kx2j8XuotCYUap1uBYRM5UWArRnfnSv0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>AQI</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1saNRhE1lTJyWSRQTbPN6nIesX0kRGOx1/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1amVihMObcBwSYfZxmxeAXNxFKbRssTFi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Small Lot First</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/16Gvn09eigAaaOKhbSdg5DJ9Bx_W5tTHV/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Matching Rule</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Zd8MrUHO1P-jSGC2izMmDDlxk3BqJw1O/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Complex Replace</t>
+  </si>
+  <si>
+    <t>Stock Investment</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/17qHF6-icxbhkcdWW6TGm4iqUiztbMpTy/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/18G-CQOFTieLXVpGkQaB3E-3rvsJKQNLY/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Seating Map</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1t8fcO-p0KzRPTC2RCLjLlpF3ABoSXFk9/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>CUENG Sport 2023</t>
+  </si>
+  <si>
+    <t>2565_3_Q1_01</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EzqYAfhvcaWUq-5EzXJwyZBHy3k4C9CK/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>2565_3_Q1_02</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1okyp4jXo4Mj19ytxDZ4KQsSRT3sTF2Mk/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ZIvSvdEIDkFNpkuv2WKutYJ76G0Ougrx/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Election</t>
+  </si>
+  <si>
+    <t>2566_1_Q2_01</t>
+  </si>
+  <si>
+    <t>2566_1_Q3_01</t>
+  </si>
+  <si>
+    <t>2566_1_Q2_02</t>
+  </si>
+  <si>
+    <t>2566_1_Q2_03</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1uZYl_y7cE_lXltvPjL7cJdszyvffykMn/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Outlier</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1I--JE-9RUlVGtxYaqCl41rCbGkQUlSiq/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Registration Data</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1wwznsnM32l3HiC4QfTj-GI3czgv0MkZQ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Eavesdrop</t>
+  </si>
+  <si>
+    <t>One Piece</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1x2IVrmVc27GaYGnEhnUbKJCNJO1p6gpi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>2566_2_Q1_01</t>
+  </si>
+  <si>
+    <t>2566_2_Q2_01</t>
+  </si>
+  <si>
+    <t>2566_2_Q3_01</t>
+  </si>
+  <si>
+    <t>2566_2_Q1_02</t>
+  </si>
+  <si>
+    <t>2566_2_Q1_03</t>
+  </si>
+  <si>
+    <t>2566_2_Q2_02</t>
+  </si>
+  <si>
+    <t>2566_2_Q2_03</t>
+  </si>
+  <si>
+    <t>2566_2_Q3_02</t>
+  </si>
+  <si>
+    <t>2566_2_Q3_03</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ybCeNooMRTp5wFQULhpAp9nw-TCpEhRa/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Poker Hands</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Nioh4BjOtLAM-bDEjh4BpvCfbAstMSAc/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QM3JjWkZ2QuDEAW3o9mUNCqXGzSTJ0gZ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Repeat Count</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EbQl9iRAR5RYoMG8uj5-foiY2b5J6Ydo/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Bad Words</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1i2hhun44grSnF-DZH80CKTKjj4O4ch3m/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Credit Points</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ftesAF-xHat6QuRv99XYFy8gNnVN-qKJ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Text Formatter</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1LF2pj8dcpoLBjUNJ0WUCw70FL3cgfXMU/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Peak 2D</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1_I8h_pHSZyKAuHf4Xf_KONQZnPnCFmD_/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Rcox7hJg5OtCnwYM4SuiiLp4fweragxh/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Hashtag Recommendation</t>
+  </si>
+  <si>
+    <t>2566_3_Q1_01</t>
+  </si>
+  <si>
+    <t>2566_3_Q2_01</t>
+  </si>
+  <si>
+    <t>2566_3_Q3_01</t>
+  </si>
+  <si>
+    <t>2566_3_Q2_02</t>
+  </si>
+  <si>
+    <t>2566_3_Q3_02</t>
+  </si>
+  <si>
+    <t>Longest Repeating Characters</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1cBzc4kXgbFXzY45q16TeEZBRyL9_7gH3/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Euro 2024</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1bA-H_dW0TDJnl-Opur5J89TMTQz0h42Z/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Euro 2024 Sub-routing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/19hJN0aOKbgJV4HOnwSkB2eyQrlpN-r_q/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Customized Grading</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1e3KDAFFtn3tNY_MHorr3GtRUzFQd2ddP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>RSP Team</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A1</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A1-W</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A2</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A3</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A2-W</t>
+  </si>
+  <si>
+    <t>2567_1_Q1_A3-W</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_A1</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_A2</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_A3</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_A2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_B1</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_B2</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_B1-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q2_B2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A1</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A2</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A3</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_B1</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_B2</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_C1</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_C2</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A1-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_A3-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_B1-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_B2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_C1-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q3_C2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q4_A2-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q4_A3-S</t>
+  </si>
+  <si>
+    <t>2567_1_Q4_B1-S</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1FA1-F6NZ_-2u46VYxLK1FhlzvqpcO5X9/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1CNrv1M8k_bTVr7CcDMwEURMhnQGlBzSb/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Compound Interest</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1w2NXIPMJdgbLTamYX4en2fHmGKXnAClv/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Image Rotation</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1VDv3WAI-swQ8CI1ndfl1iKGPUUeLMV2a/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1_OOLiYVtHnN-0h3iZ1udPz6MoPe3Xpna/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Cosine Taylor Series</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1BsL2WmqcA0Zi5Jt8rX0YuHeto6Sjdkxg/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Sequence with Ellipsis</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1oaR67Y1HE-or7eVXa--SdzR9SslRPY8P/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1tpVYDDJD990Q14XT2uEONHCwzBXefI4N/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Continued Fraction</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ubTd8JIen2MJeLl6EGGRO86ZEGh-YOYs/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Image Flip</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Rx2OWmHmJHDPIgUdRF2nwEdlr3RrBEnL/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>List Rearrangement</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1xu1O_qGHxO20ac01xD5N8_NyYTaAmBD6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Text Search</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1DyMUTyMbEAQM_3bRSgrWTzRjZ0sHP4Lr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Loan Interest</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Vx9cJXyPUt1ZQ8ffg9O-ZhJ8uTnrOsWl/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Median of Median of K</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1lgfgUbFPWHh2C0xvCvfsrskLhjylms1b/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1mB3W8l1869SFSNg3VD2y48M7X9mKk-Ny/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1MP-Vht8zederPQOsSz3z0IIsUNj98Gcf/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Jumping Bug</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1xH6vj4ppOagjY1tbTkR5sUHK3JA6TzU5/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Grader Score</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1bOT4kKkTAf6p6lZ0D9E3ZAFUwL9Drklp/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Generations</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1j19e7_1eHrJkVVQhZYDJN_IPz6V9dBTP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Text Replace</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14jrcYfblgTZ9jnNMSjJzeXOevwjzyZ8J/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>USA Election</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QRbJQGZLhat6SViEl5cG1OF3q1H2LlX7/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>The Python</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/130S4U4hoYa6hQNmiH0_6BSWmG5HP_ZOA/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1DmAZ8jdqgMcyNonBr82crODpALnPiDP-/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1CE7eYSzGfSoup-yS-8PBxiCNk4JfY2IP/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Card Score</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1cXqiNjkYF3NR1C04DxC9gApQuYIOjy5I/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Downsampling</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1NdETVe680VmxhyiD0-egVZmvii14B4il/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Card Order</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1nqz3FyUHMtr9yfLTeuW2yKcw7nzgfn4-/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Coin Change</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RaqjKrdRqYq1Q_4bk1QxuT5OdIz_muvG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Students in Course</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1dtHz7HJZBxXfQWcV1qD4toB7S1Lekbwi/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Sales Revenue</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1-AYbnJMeKUlmUY6LSnm5LZwU2DRU2UwG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>T-Score</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1h5utWIzFUcnS0tCOtFIpk-so8qWSDqZ6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>2567_2_Q1_A1</t>
+  </si>
+  <si>
+    <t>2567_2_Q1_A2</t>
+  </si>
+  <si>
+    <t>2567_2_Q1_A3</t>
+  </si>
+  <si>
+    <t>2567_2_Q2_A1</t>
+  </si>
+  <si>
+    <t>2567_2_Q2_A2</t>
+  </si>
+  <si>
+    <t>2567_2_Q2_A3</t>
+  </si>
+  <si>
+    <t>2567_2_Q2_B1</t>
+  </si>
+  <si>
+    <t>2567_2_Q2_B2</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_A1</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_A2</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_A3</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_B1</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_B2</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_C1</t>
+  </si>
+  <si>
+    <t>2567_2_Q3_C2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1f3hgd5TDKZhNo-mKpnOi-fUeMvVRQkOZ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1j7D-tr5qBp5H0i1LItXGmxd--MQF71QW/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Temperature Change</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1v0FWx0yP8K58KgW9GwB-JNcxdg_KzSO7/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Snake and Ladders</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1j65S2cZJpf_FsUE9_QZKgJipcFh5R8Xw/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1GhTOX-xn20MxpVoo8Q9_AnJzXfbU0CWA/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Lyla</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1HxprZGmq1r8nJj6YRfVJyiFnFduKlb-T/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Snake and Ladders 2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1g1L5WnvX83lrKPCAEQFQQbIM8RMDpLfe/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>List Rearragement 2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1JdGhOynEXVT9aRMdgd9qPwb9SeFidzX5/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Text Replace in File</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1jhv8c59i_6af0xRp1c9lsiRnN2mYy4hB/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13OMN41ZzzXgnYZwzrfwgXP-PRR_fNqel/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1xhNd3hF-0datqyz816erb_OIuLOHxJ79/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Red ball</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1KceParo05PeXgSq9s0pC8BPWIEBHC6El/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1JQPTF4RkH_XMh0RffyJAe--oFt2vvAsJ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Plate Extractor</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1VZzXLBxJCZVnwWJkAfcxgIwhTQsdcmev/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Connect Four</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1DckIjdZe0aP7xbSN2p3_BLqjfuZG5_QB/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Gradsons</t>
+  </si>
+  <si>
+    <t>2567_3_Q1_A0</t>
+  </si>
+  <si>
+    <t>2567_3_Q1_A1</t>
+  </si>
+  <si>
+    <t>2567_3_Q1_A2</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>2567_3_Q2_A0</t>
+  </si>
+  <si>
+    <t>2567_3_Q2_A1</t>
+  </si>
+  <si>
+    <t>2567_3_Q2_A2</t>
+  </si>
+  <si>
+    <t>2567_3_Q3_A0</t>
+  </si>
+  <si>
+    <t>2567_3_Q3_A1</t>
+  </si>
+  <si>
+    <t>2567_3_Q3_A2</t>
+  </si>
+  <si>
+    <t>2567_3_Q3_B1</t>
+  </si>
+  <si>
+    <t>2567_3_Q3_B2</t>
+  </si>
+  <si>
+    <t>2567_3_Q4_A0</t>
+  </si>
+  <si>
+    <t>2567_3_Q4_A1</t>
+  </si>
+  <si>
+    <t>2567_3_Q4_A2</t>
+  </si>
+  <si>
+    <t>2567_3_Q4_B1</t>
+  </si>
+  <si>
+    <t>2567_3_Q4_B2</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_A0</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_A1</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_A2</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_B1</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_B2</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_C1</t>
+  </si>
+  <si>
+    <t>2567_3_Q5_C2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1jdlOMDrPVgGz6oEzKVZIo2Oo1mrq2Z6T/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1cST70loS_Wfreh2mwh7RSmKwLeR216ZH/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Scout</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1UziIdhFgHbr0cqfecQvGyEAKOLts1TO6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Luxu2wqzZvYnYrAJkCIlvHvX__ANruyE/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Planting Plan</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ou_BWBzqsKbcUSy2Uxpj_3CBsDYZt-q9/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1rn2oJeFPBMSNHAICwYwckghCxUb7Coau/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Coveyer Belt</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Kmkh6j223BnjUQg9vZjQBdBVK_uOZTnC/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Reality Show</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/16O6nEM_cnqoUypfawlbL0e0T6ECHClym/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Line Arrangement</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1T2ShDXtGH-HOEdciP0aw0AweG5KzTRLo/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/121_T1Fzngp5EhFhW_bUQCUaqqSB2bIyb/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Computer Price</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/166wIhXhfHUudlgLNZJymGaIKxNRExgRG/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Most Common Alphabet</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ElOABGMUZv3X8ulf4nfeIjL0qHpD0mnp/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Student Ranking</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1wZfQ10rCUGj30mKcJNsSonx06PzO9wCc/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1pOeszxNdypPvpQTMQmdbzZTr3cbNWI9d/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Computer Price 2</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Q02DPgZGhBLSBO2v77qX7kNRvZI2Sisn/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Least Common Animals</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1TMVjvnJ1ltHH8S8_CrdAnlekX9SKm-QQ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Weather Perception</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/18QWAzO3DB4sNp6vdtzaOhEU-TFOlXEVL/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Student Grouping</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qWUIet-zn5YuB5f9ndRhYzUuGX5YOk8x/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Maximum Sales</t>
+  </si>
+  <si>
+    <t>Get Min-Max Out of 6</t>
+  </si>
+  <si>
+    <t>Interest Rate</t>
+  </si>
+  <si>
+    <t>Total Card Value</t>
+  </si>
+  <si>
+    <t>Average Grade</t>
+  </si>
+  <si>
+    <t>Move String Right Hand</t>
   </si>
 </sst>
 </file>
@@ -1816,16 +2713,16 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +2750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1867,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1900,16 +2797,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +2820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>267</v>
       </c>
@@ -1937,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>268</v>
       </c>
@@ -1951,7 +2848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>269</v>
       </c>
@@ -1965,7 +2862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>270</v>
       </c>
@@ -1979,7 +2876,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>271</v>
       </c>
@@ -1993,7 +2890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>272</v>
       </c>
@@ -2007,7 +2904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>273</v>
       </c>
@@ -2041,16 +2938,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2064,7 +2961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>288</v>
       </c>
@@ -2078,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>289</v>
       </c>
@@ -2092,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>290</v>
       </c>
@@ -2106,7 +3003,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>291</v>
       </c>
@@ -2120,7 +3017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>292</v>
       </c>
@@ -2134,7 +3031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>293</v>
       </c>
@@ -2148,7 +3045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>294</v>
       </c>
@@ -2162,7 +3059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>295</v>
       </c>
@@ -2176,7 +3073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>296</v>
       </c>
@@ -2190,7 +3087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>297</v>
       </c>
@@ -2204,7 +3101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>298</v>
       </c>
@@ -2242,16 +3139,16 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +3162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>321</v>
       </c>
@@ -2279,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>322</v>
       </c>
@@ -2293,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>323</v>
       </c>
@@ -2307,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>324</v>
       </c>
@@ -2321,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>325</v>
       </c>
@@ -2335,7 +3232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>326</v>
       </c>
@@ -2349,7 +3246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>327</v>
       </c>
@@ -2384,16 +3281,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>342</v>
       </c>
@@ -2421,7 +3318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>343</v>
       </c>
@@ -2435,7 +3332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>344</v>
       </c>
@@ -2449,7 +3346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>345</v>
       </c>
@@ -2463,7 +3360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>346</v>
       </c>
@@ -2477,7 +3374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>347</v>
       </c>
@@ -2491,7 +3388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>348</v>
       </c>
@@ -2505,7 +3402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>349</v>
       </c>
@@ -2540,16 +3437,16 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2563,7 +3460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>366</v>
       </c>
@@ -2577,7 +3474,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>367</v>
       </c>
@@ -2591,7 +3488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>368</v>
       </c>
@@ -2605,7 +3502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>369</v>
       </c>
@@ -2619,7 +3516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>370</v>
       </c>
@@ -2633,7 +3530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>371</v>
       </c>
@@ -2647,7 +3544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>372</v>
       </c>
@@ -2661,7 +3558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>373</v>
       </c>
@@ -2675,7 +3572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>374</v>
       </c>
@@ -2689,7 +3586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>375</v>
       </c>
@@ -2703,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>376</v>
       </c>
@@ -2717,13 +3614,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
     </row>
   </sheetData>
@@ -2740,16 +3637,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2763,7 +3660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>397</v>
       </c>
@@ -2777,7 +3674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>398</v>
       </c>
@@ -2791,7 +3688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>399</v>
       </c>
@@ -2805,7 +3702,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>400</v>
       </c>
@@ -2819,7 +3716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>401</v>
       </c>
@@ -2833,7 +3730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>402</v>
       </c>
@@ -2847,7 +3744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>403</v>
       </c>
@@ -2861,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>404</v>
       </c>
@@ -2875,7 +3772,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>405</v>
       </c>
@@ -2889,19 +3786,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
   </sheetData>
@@ -2914,20 +3811,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFF1BA2-EC02-4A6B-A523-8D6726D92B5D}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2941,7 +3838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>423</v>
       </c>
@@ -2955,7 +3852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>424</v>
       </c>
@@ -2969,7 +3866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>425</v>
       </c>
@@ -2983,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>426</v>
       </c>
@@ -2997,7 +3894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>427</v>
       </c>
@@ -3011,7 +3908,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>428</v>
       </c>
@@ -3025,7 +3922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>429</v>
       </c>
@@ -3039,7 +3936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>430</v>
       </c>
@@ -3053,7 +3950,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>431</v>
       </c>
@@ -3067,7 +3964,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>432</v>
       </c>
@@ -3081,13 +3978,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
   </sheetData>
@@ -3108,6 +4005,454 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82216879-8A9A-4537-803A-7E889BEBB5F7}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC4D46E-2D49-485A-8A8A-51F68404449B}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4465338-B68D-452A-8BD8-1A9919253101}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D550803-74D4-40DA-8E50-1948B5304771}">
   <dimension ref="A1:D9"/>
@@ -3116,16 +4461,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3139,7 +4484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3153,7 +4498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3167,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3181,7 +4526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3195,7 +4540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -3209,7 +4554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3223,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3237,7 +4582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -3264,6 +4609,1509 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F89C8A1-F68E-4602-9EE0-67AAE79F197D}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B7BF24-B5B9-4864-9310-52805C4B7399}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5217AF3-37F9-4125-98EB-BC53095E9B32}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3069BC-6AD1-4157-8072-BAEB9DA03623}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BAC73C-B22A-401A-B06F-4B71C95190A4}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBDC864-F75D-4D9D-9544-75FE3F6133A2}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E3ECF1-4187-4A0E-87F5-511A8C53CF19}">
   <dimension ref="A1:D12"/>
@@ -3272,16 +6120,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3295,7 +6143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -3309,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -3323,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -3337,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -3351,7 +6199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -3365,7 +6213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -3379,7 +6227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -3393,7 +6241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -3407,7 +6255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -3421,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -3435,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
@@ -3473,16 +6321,16 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3496,7 +6344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
@@ -3510,7 +6358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -3524,7 +6372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3538,7 +6386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
@@ -3552,7 +6400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -3566,7 +6414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -3580,7 +6428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3594,7 +6442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -3608,7 +6456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>78</v>
       </c>
@@ -3622,7 +6470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -3636,7 +6484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
@@ -3650,7 +6498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
@@ -3664,7 +6512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -3678,7 +6526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -3692,7 +6540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>83</v>
       </c>
@@ -3706,7 +6554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
@@ -3749,16 +6597,16 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +6620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -3786,7 +6634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -3800,7 +6648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
@@ -3814,7 +6662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -3828,7 +6676,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -3842,7 +6690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
@@ -3856,7 +6704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>124</v>
       </c>
@@ -3870,7 +6718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>125</v>
       </c>
@@ -3884,7 +6732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>126</v>
       </c>
@@ -3898,7 +6746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -3912,7 +6760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>128</v>
       </c>
@@ -3926,7 +6774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
@@ -3940,7 +6788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -3954,7 +6802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -3968,7 +6816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>132</v>
       </c>
@@ -4010,16 +6858,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +6881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>163</v>
       </c>
@@ -4047,7 +6895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>164</v>
       </c>
@@ -4061,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>165</v>
       </c>
@@ -4075,7 +6923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>166</v>
       </c>
@@ -4089,7 +6937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>167</v>
       </c>
@@ -4103,7 +6951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -4117,7 +6965,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>169</v>
       </c>
@@ -4131,7 +6979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>170</v>
       </c>
@@ -4145,7 +6993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
@@ -4159,7 +7007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>172</v>
       </c>
@@ -4173,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>173</v>
       </c>
@@ -4187,7 +7035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>174</v>
       </c>
@@ -4201,7 +7049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>175</v>
       </c>
@@ -4215,7 +7063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>176</v>
       </c>
@@ -4256,16 +7104,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4279,7 +7127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>205</v>
       </c>
@@ -4293,7 +7141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>206</v>
       </c>
@@ -4307,7 +7155,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>207</v>
       </c>
@@ -4321,7 +7169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>208</v>
       </c>
@@ -4335,7 +7183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>209</v>
       </c>
@@ -4349,7 +7197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>210</v>
       </c>
@@ -4382,16 +7230,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4405,7 +7253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>223</v>
       </c>
@@ -4419,7 +7267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>224</v>
       </c>
@@ -4433,7 +7281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>225</v>
       </c>
@@ -4447,7 +7295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>226</v>
       </c>
@@ -4461,7 +7309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>227</v>
       </c>
@@ -4475,7 +7323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>228</v>
       </c>
@@ -4489,7 +7337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>229</v>
       </c>
@@ -4503,7 +7351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>230</v>
       </c>
@@ -4538,16 +7386,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4561,7 +7409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>247</v>
       </c>
@@ -4575,7 +7423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>248</v>
       </c>
@@ -4589,7 +7437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>249</v>
       </c>
@@ -4603,7 +7451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>250</v>
       </c>
@@ -4617,7 +7465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>251</v>
       </c>
@@ -4631,7 +7479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>252</v>
       </c>
@@ -4645,7 +7493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>253</v>
       </c>

</xml_diff>